<commit_message>
Removed all .DS_Store files, Fixed git ignore and added my ideas for ants
</commit_message>
<xml_diff>
--- a/Ants.xlsx
+++ b/Ants.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15576" windowHeight="12504" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t>Species</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Barbaric</t>
   </si>
   <si>
-    <t>Odourous</t>
-  </si>
-  <si>
     <t>Hostile</t>
   </si>
   <si>
@@ -214,13 +211,28 @@
   </si>
   <si>
     <t>Produces formic acid</t>
+  </si>
+  <si>
+    <t>Acidic</t>
+  </si>
+  <si>
+    <t>Toxic</t>
+  </si>
+  <si>
+    <t>Swampland, Jungle</t>
+  </si>
+  <si>
+    <t>Cultivator + Jungle</t>
+  </si>
+  <si>
+    <t>Grows Fungi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -644,20 +656,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.69921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -671,19 +683,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>2</v>
@@ -703,7 +715,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="b">
         <v>0</v>
@@ -714,7 +726,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -726,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F3" s="4" t="b">
         <v>0</v>
@@ -749,7 +761,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -772,7 +784,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5" t="b">
         <v>0</v>
@@ -795,7 +807,7 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -806,7 +818,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="b">
         <v>1</v>
@@ -829,7 +841,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -841,7 +853,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" t="b">
         <v>0</v>
@@ -852,7 +864,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -864,7 +876,7 @@
         <v>10</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -875,7 +887,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -901,12 +913,12 @@
         <v>0</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -923,16 +935,16 @@
         <v>10</v>
       </c>
       <c r="E15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
         <v>43</v>
-      </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="b">
-        <v>0</v>
-      </c>
-      <c r="H15" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -949,21 +961,21 @@
         <v>10</v>
       </c>
       <c r="E16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>45</v>
-      </c>
-      <c r="F16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
@@ -984,12 +996,12 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="b">
         <v>0</v>
@@ -1010,12 +1022,12 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -1032,19 +1044,19 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
         <v>50</v>
       </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
-        <v>51</v>
-      </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1061,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" t="b">
         <v>0</v>
@@ -1070,15 +1082,15 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B23" t="b">
         <v>0</v>
@@ -1099,15 +1111,15 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
@@ -1128,15 +1140,15 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" t="b">
         <v>0</v>
@@ -1157,15 +1169,15 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -1186,15 +1198,15 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
@@ -1215,15 +1227,15 @@
         <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B28" t="b">
         <v>0</v>
@@ -1235,7 +1247,7 @@
         <v>10</v>
       </c>
       <c r="E28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F28" t="b">
         <v>0</v>
@@ -1244,10 +1256,39 @@
         <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I28" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>